<commit_message>
fix: Allow birthdate authentication after PIN setup for seamless application flow
- 문제: 생년월일 로그인 → PIN 설정 → 로그아웃 없이 신청 시 "Invalid PIN" 오류
- 해결: submit-v3 API에서 PIN 설정된 직원도 생년월일 인증 허용 (세션 유지)
- 로그인은 여전히 엄격 (PIN 설정 시 PIN만 허용)
- 보안: 로그인 단계에서 검증, 신청은 유연하게 처리

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/직원등록_템플릿.xlsx
+++ b/docs/직원등록_템플릿.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\작업\프로그램 만들기\연세바로치과 스케줄러\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="525" windowWidth="27735" windowHeight="11925"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="46">
   <si>
     <t>이름</t>
   </si>
@@ -150,22 +145,25 @@
     <t>유연배치구분</t>
   </si>
   <si>
-    <t>유연배치우선순위</t>
-  </si>
-  <si>
     <t>저년차</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>고년차,저년차</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>총연차</t>
+  </si>
+  <si>
+    <t>사용연차</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -541,24 +539,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
     <col min="2" max="2" width="12.77734375" customWidth="1"/>
     <col min="3" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="10.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,13 +575,16 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -604,7 +604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -624,7 +624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -643,11 +643,11 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -663,11 +663,11 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -683,11 +683,11 @@
       <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -703,11 +703,11 @@
       <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -723,11 +723,11 @@
       <c r="F8" t="s">
         <v>8</v>
       </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -743,11 +743,11 @@
       <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -763,11 +763,11 @@
       <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -783,11 +783,11 @@
       <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="G11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -803,11 +803,11 @@
       <c r="F12" t="s">
         <v>8</v>
       </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -823,11 +823,11 @@
       <c r="F13" t="s">
         <v>8</v>
       </c>
-      <c r="G13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -843,11 +843,11 @@
       <c r="F14" t="s">
         <v>8</v>
       </c>
-      <c r="G14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -863,11 +863,11 @@
       <c r="F15" t="s">
         <v>8</v>
       </c>
-      <c r="G15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -883,11 +883,11 @@
       <c r="F16" t="s">
         <v>8</v>
       </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -903,11 +903,11 @@
       <c r="F17" t="s">
         <v>8</v>
       </c>
-      <c r="G17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -918,13 +918,13 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -941,7 +941,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -958,7 +958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -975,7 +975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -989,7 +989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
fix: Change staff-bulk API to UPDATE-only (no DELETE) and send only modified staff
- API: Remove deleteMany, use UPDATE for existing staff
- Frontend: Track original data, send only modified staff
- Fix: pin -> pinCode field name
- Fix: Leave application bulk submit - exclude successful dates from otherSelectedDates
- Fix: Doctor schedule deletion clears weekPatterns
- Fix: Doctor summary returns correct hasSchedule based on actual data
- UI: Differentiate leave type colors in selection list

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/직원등록_템플릿.xlsx
+++ b/docs/직원등록_템플릿.xlsx
@@ -543,7 +543,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -912,7 +912,7 @@
         <v>28</v>
       </c>
       <c r="B18">
-        <v>960230</v>
+        <v>960222</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -929,7 +929,7 @@
         <v>30</v>
       </c>
       <c r="B19">
-        <v>960231</v>
+        <v>960229</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -946,7 +946,7 @@
         <v>31</v>
       </c>
       <c r="B20">
-        <v>960232</v>
+        <v>960211</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -963,7 +963,7 @@
         <v>32</v>
       </c>
       <c r="B21">
-        <v>960233</v>
+        <v>960203</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -980,7 +980,7 @@
         <v>33</v>
       </c>
       <c r="B22">
-        <v>960234</v>
+        <v>960203</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -994,7 +994,7 @@
         <v>34</v>
       </c>
       <c r="B23">
-        <v>960235</v>
+        <v>960205</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -1008,7 +1008,7 @@
         <v>35</v>
       </c>
       <c r="B24">
-        <v>960236</v>
+        <v>960206</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -1022,7 +1022,7 @@
         <v>36</v>
       </c>
       <c r="B25">
-        <v>960237</v>
+        <v>960207</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -1036,7 +1036,7 @@
         <v>37</v>
       </c>
       <c r="B26">
-        <v>960238</v>
+        <v>960208</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>

</xml_diff>